<commit_message>
added a function to the player to set the next card to be active added a function to give every player 8 random cards added code to remove and add cards after comparing them added a function to refresh the text on labels added a lable to display the cards currently on the hand added a cardindex variable to the playcard class
changed code to compare the active players cards
changed the layout to be easier to understand
</commit_message>
<xml_diff>
--- a/Quartett_Data/Cars.xlsx
+++ b/Quartett_Data/Cars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Quartett_Projekt\Quartett_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3106441C-B0CD-4FF0-AF7E-126A13E614F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F12646F-D2D6-4656-9ACC-AAFFAD82F157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F6C2CEED-2A88-46A8-9233-EF29B5FFF59B}"/>
   </bookViews>
@@ -507,9 +507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3275E62-2AF6-42B1-B641-95B012F20C15}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>